<commit_message>
Advect with transports/depth + swimming
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21540" yWindow="460" windowWidth="16240" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="21540" yWindow="460" windowWidth="16240" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Case</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>New 200m avg vel, dt = 1 hr, swim to random changing max</t>
+  </si>
+  <si>
+    <t>New 200m transport / depth</t>
   </si>
 </sst>
 </file>
@@ -159,7 +162,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -274,7 +277,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -563,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -830,88 +833,102 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B15" s="8">
-        <v>-3.5659999999999998</v>
+        <v>-2.4333999999999998</v>
       </c>
       <c r="C15" s="8">
-        <v>-0.5968</v>
+        <v>0.39710000000000001</v>
       </c>
       <c r="D15" s="8">
-        <v>-10.3956</v>
+        <v>-1.4021999999999999</v>
       </c>
       <c r="E15" s="8">
-        <v>-2.4392</v>
+        <v>0.90859999999999996</v>
       </c>
       <c r="F15" s="8">
-        <v>4.7607999999999997</v>
+        <v>-0.23330000000000001</v>
       </c>
       <c r="G15" s="8">
-        <v>-4.1600999999999999</v>
+        <v>-0.3029</v>
       </c>
       <c r="H15" s="8">
-        <v>-2.0428999999999999</v>
+        <v>-0.14630000000000001</v>
       </c>
       <c r="I15" s="8">
-        <v>-0.38080000000000003</v>
+        <v>7.0800000000000002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="8">
-        <v>-4.9553000000000003</v>
-      </c>
-      <c r="C16" s="9">
-        <v>6.1597E+18</v>
+        <v>-3.5659999999999998</v>
+      </c>
+      <c r="C16" s="8">
+        <v>-0.5968</v>
       </c>
       <c r="D16" s="8">
-        <v>-13.9963</v>
-      </c>
-      <c r="E16" s="9">
-        <v>3.4736999999999997E+45</v>
+        <v>-10.3956</v>
+      </c>
+      <c r="E16" s="8">
+        <v>-2.4392</v>
       </c>
       <c r="F16" s="8">
-        <v>-2.9847000000000001</v>
-      </c>
-      <c r="G16" s="10">
-        <v>-4.5688000000000004</v>
+        <v>4.7607999999999997</v>
+      </c>
+      <c r="G16" s="8">
+        <v>-4.1600999999999999</v>
       </c>
       <c r="H16" s="8">
-        <v>-1.6102000000000001</v>
-      </c>
-      <c r="I16" s="9">
-        <v>2.8743999999999999E+44</v>
+        <v>-2.0428999999999999</v>
+      </c>
+      <c r="I16" s="8">
+        <v>-0.38080000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6">
-        <v>-2.4392</v>
-      </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="B17" s="8">
+        <v>-4.9553000000000003</v>
+      </c>
+      <c r="C17" s="9">
+        <v>6.1597E+18</v>
+      </c>
+      <c r="D17" s="8">
+        <v>-13.9963</v>
+      </c>
+      <c r="E17" s="9">
+        <v>3.4736999999999997E+45</v>
+      </c>
+      <c r="F17" s="8">
+        <v>-2.9847000000000001</v>
+      </c>
+      <c r="G17" s="10">
+        <v>-4.5688000000000004</v>
+      </c>
+      <c r="H17" s="8">
+        <v>-1.6102000000000001</v>
+      </c>
+      <c r="I17" s="9">
+        <v>2.8743999999999999E+44</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="7">
-        <v>3.4736999999999997E+45</v>
+      <c r="E18" s="6">
+        <v>-2.4392</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -920,112 +937,127 @@
     </row>
     <row r="19" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="6"/>
-      <c r="C19" s="7">
-        <v>2.6601999999999998E+37</v>
-      </c>
+      <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="7">
-        <v>3.1471000000000002E+46</v>
+        <v>3.4736999999999997E+45</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="7">
-        <v>1.5424999999999999E+42</v>
-      </c>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="6">
-        <v>4.7473000000000001</v>
+      <c r="C20" s="7">
+        <v>2.6601999999999998E+37</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6">
-        <v>161.745</v>
+      <c r="E20" s="7">
+        <v>3.1471000000000002E+46</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="6">
+      <c r="I20" s="7">
+        <v>1.5424999999999999E+42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6">
+        <v>4.7473000000000001</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6">
+        <v>161.745</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6">
         <v>177.05170000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="1">
-        <v>5.7000000000000005E+95</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B42" s="1">
-        <v>1.2E+106</v>
+        <v>5.7000000000000005E+95</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B43" s="1">
-        <v>4.4000000000000004E+93</v>
+        <v>1.2E+106</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B44" s="1">
-        <v>2700000000</v>
+        <v>4.4000000000000004E+93</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B45" s="1">
-        <v>91000000</v>
+        <v>2700000000</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" s="1">
-        <v>2500</v>
+        <v>91000000</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B48" s="1">
         <v>9.5999999999999996E+83</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C48" s="1">
         <v>1.2999999999999999E+24</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D48" s="1">
         <v>4.6000000000000003E+93</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E48" s="1">
         <v>7.4999999999999994E+29</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F48" s="1">
         <v>37.9</v>
       </c>
     </row>
@@ -1038,7 +1070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Use transports divide by depth(i,j) in function
Instead of dividing by depth before calling advection, divide by depth
when calculating the tendency.
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21540" yWindow="460" windowWidth="16240" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="12620" yWindow="460" windowWidth="16240" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Case</t>
   </si>
@@ -153,7 +153,19 @@
     <t>New 200m avg vel, dt = 1 hr, swim to random changing max</t>
   </si>
   <si>
-    <t>New 200m transport / depth</t>
+    <t>New 200m transport / depth, dt = 1 hr, j = 2, swim to shallow</t>
+  </si>
+  <si>
+    <t>New 200m transport / depth, dt = 1 hr, j = 2, swim to deep</t>
+  </si>
+  <si>
+    <t>New 200m transport / depth, dt = 1 hr, j = 2</t>
+  </si>
+  <si>
+    <t>New 200m transport / depth, dt = 1 hr, j = 2, swim to const rand</t>
+  </si>
+  <si>
+    <t>New 200m transport / depth, dt = 1 hr, j = 2, swim to changing rand</t>
   </si>
 </sst>
 </file>
@@ -568,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -835,7 +847,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B15" s="8">
         <v>-2.4333999999999998</v>
@@ -986,6 +998,74 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6">
         <v>177.05170000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6">
+        <v>0.33189999999999997</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6">
+        <v>15.1043</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6">
+        <v>2.1004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7">
+        <v>7470400000</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7">
+        <v>6.6192999999999997E+46</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="7">
+        <v>5.4772000000000002E+45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="7">
+        <v>2.2199000000000001E+46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6">
+        <v>44.083599999999997</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Test diff benthic efficiencies
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12620" yWindow="460" windowWidth="16240" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="21540" yWindow="460" windowWidth="16240" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Case</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>New 200m transport / depth, dt = 1 hr, j = 2, swim to changing rand</t>
+  </si>
+  <si>
+    <t>New 200m transport,  flux/depth, dt = 1 hr, j = 2</t>
   </si>
 </sst>
 </file>
@@ -578,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -876,86 +879,100 @@
     </row>
     <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B16" s="8">
-        <v>-3.5659999999999998</v>
+        <v>-4.5010000000000003</v>
       </c>
       <c r="C16" s="8">
-        <v>-0.5968</v>
+        <v>-1.5115000000000001</v>
       </c>
       <c r="D16" s="8">
-        <v>-10.3956</v>
+        <v>-1.7454000000000001</v>
       </c>
       <c r="E16" s="8">
-        <v>-2.4392</v>
+        <v>-2.09</v>
       </c>
       <c r="F16" s="8">
-        <v>4.7607999999999997</v>
+        <v>0.94450000000000001</v>
       </c>
       <c r="G16" s="8">
-        <v>-4.1600999999999999</v>
+        <v>-0.66759999999999997</v>
       </c>
       <c r="H16" s="8">
-        <v>-2.0428999999999999</v>
+        <v>0.44950000000000001</v>
       </c>
       <c r="I16" s="8">
-        <v>-0.38080000000000003</v>
+        <v>-0.1013</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="8">
-        <v>-4.9553000000000003</v>
-      </c>
-      <c r="C17" s="9">
-        <v>6.1597E+18</v>
+        <v>-3.5659999999999998</v>
+      </c>
+      <c r="C17" s="8">
+        <v>-0.5968</v>
       </c>
       <c r="D17" s="8">
-        <v>-13.9963</v>
-      </c>
-      <c r="E17" s="9">
-        <v>3.4736999999999997E+45</v>
+        <v>-10.3956</v>
+      </c>
+      <c r="E17" s="8">
+        <v>-2.4392</v>
       </c>
       <c r="F17" s="8">
-        <v>-2.9847000000000001</v>
-      </c>
-      <c r="G17" s="10">
-        <v>-4.5688000000000004</v>
+        <v>4.7607999999999997</v>
+      </c>
+      <c r="G17" s="8">
+        <v>-4.1600999999999999</v>
       </c>
       <c r="H17" s="8">
-        <v>-1.6102000000000001</v>
-      </c>
-      <c r="I17" s="9">
-        <v>2.8743999999999999E+44</v>
+        <v>-2.0428999999999999</v>
+      </c>
+      <c r="I17" s="8">
+        <v>-0.38080000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6">
-        <v>-2.4392</v>
-      </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="B18" s="8">
+        <v>-4.9553000000000003</v>
+      </c>
+      <c r="C18" s="9">
+        <v>6.1597E+18</v>
+      </c>
+      <c r="D18" s="8">
+        <v>-13.9963</v>
+      </c>
+      <c r="E18" s="9">
+        <v>3.4736999999999997E+45</v>
+      </c>
+      <c r="F18" s="8">
+        <v>-2.9847000000000001</v>
+      </c>
+      <c r="G18" s="10">
+        <v>-4.5688000000000004</v>
+      </c>
+      <c r="H18" s="8">
+        <v>-1.6102000000000001</v>
+      </c>
+      <c r="I18" s="9">
+        <v>2.8743999999999999E+44</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="7">
-        <v>3.4736999999999997E+45</v>
+      <c r="E19" s="6">
+        <v>-2.4392</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -964,98 +981,98 @@
     </row>
     <row r="20" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="7">
-        <v>2.6601999999999998E+37</v>
-      </c>
+      <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="7">
-        <v>3.1471000000000002E+46</v>
+        <v>3.4736999999999997E+45</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="7">
-        <v>1.5424999999999999E+42</v>
-      </c>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="6">
-        <v>4.7473000000000001</v>
+      <c r="C21" s="7">
+        <v>2.6601999999999998E+37</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="6">
-        <v>161.745</v>
+      <c r="E21" s="7">
+        <v>3.1471000000000002E+46</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="6">
-        <v>177.05170000000001</v>
+      <c r="I21" s="7">
+        <v>1.5424999999999999E+42</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6">
-        <v>0.33189999999999997</v>
+        <v>4.7473000000000001</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6">
-        <v>15.1043</v>
+        <v>161.745</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6">
-        <v>2.1004</v>
+        <v>177.05170000000001</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="7">
-        <v>7470400000</v>
+      <c r="C23" s="6">
+        <v>0.33189999999999997</v>
       </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="7">
-        <v>6.6192999999999997E+46</v>
+      <c r="E23" s="6">
+        <v>15.1043</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="7">
-        <v>5.4772000000000002E+45</v>
+      <c r="I23" s="6">
+        <v>2.1004</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
+      <c r="C24" s="7">
+        <v>7470400000</v>
+      </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="E24" s="7">
+        <v>6.6192999999999997E+46</v>
+      </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="7">
-        <v>2.2199000000000001E+46</v>
+        <v>5.4772000000000002E+45</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1064,80 +1081,95 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="6">
+      <c r="I25" s="7">
+        <v>2.2199000000000001E+46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6">
         <v>44.083599999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B43" s="1">
         <v>5.7000000000000005E+95</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B44" s="1">
         <v>1.2E+106</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B45" s="1">
         <v>4.4000000000000004E+93</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B46" s="1">
         <v>2700000000</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B47" s="1">
         <v>91000000</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B48" s="1">
         <v>2500</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B49" s="1">
         <v>9.5999999999999996E+83</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C49" s="1">
         <v>1.2999999999999999E+24</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D49" s="1">
         <v>4.6000000000000003E+93</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E49" s="1">
         <v>7.4999999999999994E+29</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F49" s="1">
         <v>37.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mizer & J&C nmort w/fishing
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21540" yWindow="460" windowWidth="16240" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="13440" yWindow="460" windowWidth="24720" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$16</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -255,7 +258,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -301,6 +304,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -581,22 +590,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="15" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
+    <col min="3" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="11" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -604,12 +616,12 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -617,564 +629,636 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8">
+      <c r="C4" s="18">
         <v>-7.8666</v>
       </c>
-      <c r="C4" s="8">
+      <c r="D4" s="18">
         <v>-5.3753000000000002</v>
       </c>
-      <c r="D4" s="8">
+      <c r="E4" s="18">
         <v>-20.837299999999999</v>
       </c>
-      <c r="E4" s="8">
+      <c r="F4" s="18">
         <v>-0.31740000000000002</v>
       </c>
-      <c r="F4" s="8">
+      <c r="G4" s="18">
         <v>-5.1647999999999996</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8">
+      <c r="H4" s="18"/>
+      <c r="I4" s="18">
         <v>-6.4858000000000002</v>
       </c>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8">
+      <c r="C5" s="18">
         <v>-15.323700000000001</v>
       </c>
-      <c r="C5" s="8">
+      <c r="D5" s="18">
         <v>-12.789099999999999</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8">
+      <c r="C6" s="18">
         <v>-4.3329000000000004</v>
       </c>
-      <c r="C6" s="8">
+      <c r="D6" s="18">
         <v>1.6291</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8">
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18">
         <v>-4.7885</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="18">
         <v>0.49940000000000001</v>
       </c>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="9">
+      <c r="H7" s="8"/>
+      <c r="I7" s="9">
         <v>-8.6800999999999995E-7</v>
       </c>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8">
+      <c r="C8" s="18">
         <v>23.395</v>
       </c>
-      <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8">
+      <c r="C9" s="18">
         <v>23.395</v>
       </c>
-      <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="15">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8">
+      <c r="C10" s="18">
         <v>23.412199999999999</v>
       </c>
-      <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="15">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="8">
+      <c r="C11" s="18">
         <v>-4.3</v>
       </c>
-      <c r="C11" s="8">
+      <c r="D11" s="18">
         <v>1.6</v>
       </c>
-      <c r="D11" s="8">
+      <c r="E11" s="18">
         <v>-11.5</v>
       </c>
-      <c r="E11" s="8">
+      <c r="F11" s="18">
         <v>-0.8</v>
       </c>
-      <c r="F11" s="8">
+      <c r="G11" s="18">
         <v>-2.5</v>
       </c>
-      <c r="G11" s="8">
+      <c r="H11" s="18">
         <v>-4.2</v>
       </c>
-      <c r="H11" s="8">
+      <c r="I11" s="18">
         <v>-0.5</v>
       </c>
-      <c r="I11" s="8">
+      <c r="J11" s="18">
         <v>-1.3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="15">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="8">
+      <c r="C12" s="18">
         <v>-4.3</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="15">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18">
         <v>-1.2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="15">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="8">
+      <c r="C14" s="18">
         <v>-4.3</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="8">
+      <c r="C15" s="18">
         <v>-2.4333999999999998</v>
       </c>
-      <c r="C15" s="8">
+      <c r="D15" s="18">
         <v>0.39710000000000001</v>
       </c>
-      <c r="D15" s="8">
+      <c r="E15" s="18">
         <v>-1.4021999999999999</v>
       </c>
-      <c r="E15" s="8">
+      <c r="F15" s="18">
         <v>0.90859999999999996</v>
       </c>
-      <c r="F15" s="8">
+      <c r="G15" s="18">
         <v>-0.23330000000000001</v>
       </c>
-      <c r="G15" s="8">
+      <c r="H15" s="18">
         <v>-0.3029</v>
       </c>
-      <c r="H15" s="8">
+      <c r="I15" s="18">
         <v>-0.14630000000000001</v>
       </c>
-      <c r="I15" s="8">
+      <c r="J15" s="18">
         <v>7.0800000000000002E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="15">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="8">
+      <c r="C16" s="18">
         <v>-4.5010000000000003</v>
       </c>
-      <c r="C16" s="8">
+      <c r="D16" s="18">
         <v>-1.5115000000000001</v>
       </c>
-      <c r="D16" s="8">
+      <c r="E16" s="18">
         <v>-1.7454000000000001</v>
       </c>
-      <c r="E16" s="8">
+      <c r="F16" s="18">
         <v>-2.09</v>
       </c>
-      <c r="F16" s="8">
+      <c r="G16" s="18">
         <v>0.94450000000000001</v>
       </c>
-      <c r="G16" s="8">
+      <c r="H16" s="18">
         <v>-0.66759999999999997</v>
       </c>
-      <c r="H16" s="8">
+      <c r="I16" s="18">
         <v>0.44950000000000001</v>
       </c>
-      <c r="I16" s="8">
+      <c r="J16" s="18">
         <v>-0.1013</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="15">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="8">
+      <c r="C17" s="18">
         <v>-3.5659999999999998</v>
       </c>
-      <c r="C17" s="8">
+      <c r="D17" s="18">
         <v>-0.5968</v>
       </c>
-      <c r="D17" s="8">
+      <c r="E17" s="18">
         <v>-10.3956</v>
       </c>
-      <c r="E17" s="8">
+      <c r="F17" s="18">
         <v>-2.4392</v>
       </c>
-      <c r="F17" s="8">
+      <c r="G17" s="18">
         <v>4.7607999999999997</v>
       </c>
-      <c r="G17" s="8">
+      <c r="H17" s="18">
         <v>-4.1600999999999999</v>
       </c>
-      <c r="H17" s="8">
+      <c r="I17" s="18">
         <v>-2.0428999999999999</v>
       </c>
-      <c r="I17" s="8">
+      <c r="J17" s="18">
         <v>-0.38080000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="15">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="8">
+      <c r="C18" s="18">
         <v>-4.9553000000000003</v>
       </c>
-      <c r="C18" s="9">
+      <c r="D18" s="9">
         <v>6.1597E+18</v>
       </c>
-      <c r="D18" s="8">
+      <c r="E18" s="8">
         <v>-13.9963</v>
       </c>
-      <c r="E18" s="9">
+      <c r="F18" s="9">
         <v>3.4736999999999997E+45</v>
       </c>
-      <c r="F18" s="8">
+      <c r="G18" s="8">
         <v>-2.9847000000000001</v>
       </c>
-      <c r="G18" s="10">
+      <c r="H18" s="10">
         <v>-4.5688000000000004</v>
       </c>
-      <c r="H18" s="8">
+      <c r="I18" s="8">
         <v>-1.6102000000000001</v>
       </c>
-      <c r="I18" s="9">
+      <c r="J18" s="9">
         <v>2.8743999999999999E+44</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="15">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="6">
+      <c r="E19" s="6"/>
+      <c r="F19" s="19">
         <v>-2.4392</v>
       </c>
-      <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="7">
+      <c r="E20" s="6"/>
+      <c r="F20" s="7">
         <v>3.4736999999999997E+45</v>
       </c>
-      <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="15">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7">
+      <c r="C21" s="6"/>
+      <c r="D21" s="7">
         <v>2.6601999999999998E+37</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7">
+      <c r="E21" s="6"/>
+      <c r="F21" s="7">
         <v>3.1471000000000002E+46</v>
       </c>
-      <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="7">
+      <c r="I21" s="6"/>
+      <c r="J21" s="7">
         <v>1.5424999999999999E+42</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="15">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6">
+      <c r="C22" s="6"/>
+      <c r="D22" s="19">
         <v>4.7473000000000001</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6">
+      <c r="E22" s="19"/>
+      <c r="F22" s="19">
         <v>161.745</v>
       </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6">
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19">
         <v>177.05170000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="15">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6">
+      <c r="C23" s="6"/>
+      <c r="D23" s="19">
         <v>0.33189999999999997</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6">
+      <c r="E23" s="19"/>
+      <c r="F23" s="19">
         <v>15.1043</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6">
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19">
         <v>2.1004</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="15">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7">
+      <c r="C24" s="6"/>
+      <c r="D24" s="7">
         <v>7470400000</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7">
+      <c r="E24" s="6"/>
+      <c r="F24" s="7">
         <v>6.6192999999999997E+46</v>
       </c>
-      <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="7">
+      <c r="I24" s="6"/>
+      <c r="J24" s="7">
         <v>5.4772000000000002E+45</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="15">
+        <v>22</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="7">
+      <c r="I25" s="6"/>
+      <c r="J25" s="7">
         <v>2.2199000000000001E+46</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="15">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="6">
+      <c r="I26" s="6"/>
+      <c r="J26" s="19">
         <v>44.083599999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="1">
+      <c r="C43" s="1">
         <v>5.7000000000000005E+95</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="1">
+      <c r="C44" s="1">
         <v>1.2E+106</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="1">
+      <c r="C45" s="1">
         <v>4.4000000000000004E+93</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="1">
+      <c r="C46" s="1">
         <v>2700000000</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B47" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="1">
+      <c r="C47" s="1">
         <v>91000000</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B48" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="1">
+      <c r="C48" s="1">
         <v>2500</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="1">
+      <c r="C49" s="1">
         <v>9.5999999999999996E+83</v>
       </c>
-      <c r="C49" s="1">
+      <c r="D49" s="1">
         <v>1.2999999999999999E+24</v>
       </c>
-      <c r="D49" s="1">
+      <c r="E49" s="1">
         <v>4.6000000000000003E+93</v>
       </c>
-      <c r="E49" s="1">
+      <c r="F49" s="1">
         <v>7.4999999999999994E+29</v>
       </c>
-      <c r="F49" s="1">
+      <c r="G49" s="1">
         <v>37.9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Advect trans/dep in flux calc
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="460" windowWidth="24720" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="21660" yWindow="460" windowWidth="16740" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$12:$J$27</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>Case</t>
   </si>
@@ -172,6 +173,39 @@
   </si>
   <si>
     <t>New 200m transport,  flux/depth, dt = 1 hr, j = 2</t>
+  </si>
+  <si>
+    <t>New 200m transport,  vel/depth in flux calc, dt = 1 hr, j = 2</t>
+  </si>
+  <si>
+    <t>New 200m transport,  vel/depth in flux calc, dt = 1 hr, j = 2, swim to deep</t>
+  </si>
+  <si>
+    <t>New 200m transport,  vel/depth in flux calc, dt = 1 hr, j = 2, swim to shallow</t>
+  </si>
+  <si>
+    <t>Pure advection cases</t>
+  </si>
+  <si>
+    <t>Advection + swimming cases</t>
+  </si>
+  <si>
+    <t>Swimming only cases</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 1 hr, j = 2, swim to shallow</t>
+  </si>
+  <si>
+    <t>Zero advec vel,  vel/depth in flux calc, dt = 1 hr, j = 2, swim to deep</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Old-12</t>
+  </si>
+  <si>
+    <t>Old-13</t>
   </si>
 </sst>
 </file>
@@ -236,12 +270,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -258,7 +298,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -309,6 +349,18 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -590,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -959,299 +1011,445 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="15">
-        <v>14</v>
+      <c r="A17" s="21">
+        <v>24</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="18">
-        <v>-3.5659999999999998</v>
-      </c>
-      <c r="D17" s="18">
-        <v>-0.5968</v>
+        <v>47</v>
+      </c>
+      <c r="C17" s="20">
+        <v>-1.9511000000000001</v>
+      </c>
+      <c r="D17" s="19">
+        <v>0.40229999999999999</v>
       </c>
       <c r="E17" s="18">
-        <v>-10.3956</v>
+        <v>-1.2970999999999999</v>
       </c>
       <c r="F17" s="18">
-        <v>-2.4392</v>
+        <v>0.60670000000000002</v>
       </c>
       <c r="G17" s="18">
-        <v>4.7607999999999997</v>
+        <v>-0.27260000000000001</v>
       </c>
       <c r="H17" s="18">
-        <v>-4.1600999999999999</v>
+        <v>-0.33079999999999998</v>
       </c>
       <c r="I17" s="18">
-        <v>-2.0428999999999999</v>
+        <v>-0.15629999999999999</v>
       </c>
       <c r="J17" s="18">
-        <v>-0.38080000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="15">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="18">
-        <v>-4.9553000000000003</v>
-      </c>
-      <c r="D18" s="9">
-        <v>6.1597E+18</v>
-      </c>
-      <c r="E18" s="8">
-        <v>-13.9963</v>
-      </c>
-      <c r="F18" s="9">
-        <v>3.4736999999999997E+45</v>
-      </c>
-      <c r="G18" s="8">
-        <v>-2.9847000000000001</v>
-      </c>
-      <c r="H18" s="10">
-        <v>-4.5688000000000004</v>
-      </c>
-      <c r="I18" s="8">
-        <v>-1.6102000000000001</v>
-      </c>
-      <c r="J18" s="9">
-        <v>2.8743999999999999E+44</v>
-      </c>
+        <v>-9.2799999999999994E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="19">
+        <v>30</v>
+      </c>
+      <c r="C19" s="18">
+        <v>-3.5659999999999998</v>
+      </c>
+      <c r="D19" s="18">
+        <v>-0.5968</v>
+      </c>
+      <c r="E19" s="18">
+        <v>-10.3956</v>
+      </c>
+      <c r="F19" s="18">
         <v>-2.4392</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+      <c r="G19" s="18">
+        <v>4.7607999999999997</v>
+      </c>
+      <c r="H19" s="18">
+        <v>-4.1600999999999999</v>
+      </c>
+      <c r="I19" s="18">
+        <v>-2.0428999999999999</v>
+      </c>
+      <c r="J19" s="18">
+        <v>-0.38080000000000003</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7">
+        <v>31</v>
+      </c>
+      <c r="C20" s="18">
+        <v>-4.9553000000000003</v>
+      </c>
+      <c r="D20" s="9">
+        <v>6.1597E+18</v>
+      </c>
+      <c r="E20" s="8">
+        <v>-13.9963</v>
+      </c>
+      <c r="F20" s="9">
         <v>3.4736999999999997E+45</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
+      <c r="G20" s="8">
+        <v>-2.9847000000000001</v>
+      </c>
+      <c r="H20" s="10">
+        <v>-4.5688000000000004</v>
+      </c>
+      <c r="I20" s="8">
+        <v>-1.6102000000000001</v>
+      </c>
+      <c r="J20" s="9">
+        <v>2.8743999999999999E+44</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="6"/>
-      <c r="D21" s="7">
-        <v>2.6601999999999998E+37</v>
-      </c>
+      <c r="D21" s="6"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="7">
-        <v>3.1471000000000002E+46</v>
+      <c r="F21" s="19">
+        <v>-2.4392</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="7">
-        <v>1.5424999999999999E+42</v>
-      </c>
+      <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" s="6"/>
-      <c r="D22" s="19">
-        <v>4.7473000000000001</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19">
-        <v>161.745</v>
-      </c>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19">
-        <v>177.05170000000001</v>
-      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7">
+        <v>3.4736999999999997E+45</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="15">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="19">
-        <v>0.33189999999999997</v>
-      </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19">
-        <v>15.1043</v>
-      </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19">
-        <v>2.1004</v>
+      <c r="D23" s="7">
+        <v>2.6601999999999998E+37</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7">
+        <v>3.1471000000000002E+46</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="7">
+        <v>1.5424999999999999E+42</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="15">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C24" s="6"/>
-      <c r="D24" s="7">
-        <v>7470400000</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7">
-        <v>6.6192999999999997E+46</v>
-      </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="7">
-        <v>5.4772000000000002E+45</v>
+      <c r="D24" s="19">
+        <v>4.7473000000000001</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19">
+        <v>161.745</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19">
+        <v>177.05170000000001</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="15">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="7">
-        <v>2.2199000000000001E+46</v>
+      <c r="D25" s="19">
+        <v>0.33189999999999997</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19">
+        <v>15.1043</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19">
+        <v>2.1004</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="15">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+      <c r="D26" s="7">
+        <v>7470400000</v>
+      </c>
       <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="F26" s="7">
+        <v>6.6192999999999997E+46</v>
+      </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="19">
+      <c r="J26" s="7">
+        <v>5.4772000000000002E+45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="15">
+        <v>22</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="7">
+        <v>2.2199000000000001E+46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="15">
+        <v>23</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="19">
         <v>44.083599999999997</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B42" s="3" t="s">
+    <row r="29" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="21">
+        <v>25</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="19">
+        <v>-1.8743000000000001</v>
+      </c>
+      <c r="D29" s="19">
+        <v>0.29830000000000001</v>
+      </c>
+      <c r="E29" s="19">
+        <v>-1.2559</v>
+      </c>
+      <c r="F29" s="19">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="G29" s="19">
+        <v>-0.27429999999999999</v>
+      </c>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19">
+        <v>-0.12920000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="21">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="19">
+        <v>-2.0024000000000002</v>
+      </c>
+      <c r="D30" s="19">
+        <v>0.47420000000000001</v>
+      </c>
+      <c r="E30" s="19">
+        <v>-1.3398000000000001</v>
+      </c>
+      <c r="F30" s="19">
+        <v>0.57679999999999998</v>
+      </c>
+      <c r="G30" s="19">
+        <v>-0.31090000000000001</v>
+      </c>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19">
+        <v>-0.11890000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="21">
+        <v>27</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="19">
+        <v>-2.0199999999999999E-2</v>
+      </c>
+      <c r="E34" s="19">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="F34" s="19">
+        <v>1.5696000000000001</v>
+      </c>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19">
+        <v>0.82250000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="21">
+        <v>28</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19">
+        <v>0.34549999999999997</v>
+      </c>
+      <c r="E35" s="19">
+        <v>-2.5206</v>
+      </c>
+      <c r="F35" s="19">
+        <v>212.93270000000001</v>
+      </c>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19">
+        <v>16.874300000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B43" s="2" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C46" s="1">
         <v>5.7000000000000005E+95</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B44" s="2" t="s">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C47" s="1">
         <v>1.2E+106</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B45" s="2" t="s">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C48" s="1">
         <v>4.4000000000000004E+93</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="1">
-        <v>2700000000</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B47" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="1">
-        <v>91000000</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B48" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="1">
-        <v>2500</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2700000000</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="1">
+        <v>91000000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C52" s="1">
         <v>9.5999999999999996E+83</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D52" s="1">
         <v>1.2999999999999999E+24</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E52" s="1">
         <v>4.6000000000000003E+93</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F52" s="1">
         <v>7.4999999999999994E+29</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G52" s="1">
         <v>37.9</v>
       </c>
     </row>
@@ -1264,207 +1462,513 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A12" sqref="A12:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="B1" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="H3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="I3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="J3" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="13">
+      <c r="C4" s="13">
         <v>-7.8666</v>
       </c>
-      <c r="C4" s="13">
+      <c r="D4" s="13">
         <v>-5.3753000000000002</v>
       </c>
-      <c r="D4" s="13">
+      <c r="E4" s="13">
         <v>-20.837299999999999</v>
       </c>
-      <c r="E4" s="13">
+      <c r="F4" s="13">
         <v>-0.31740000000000002</v>
       </c>
-      <c r="F4" s="13">
+      <c r="G4" s="13">
         <v>-5.1647999999999996</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
         <v>-6.4858000000000002</v>
       </c>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="13">
+      <c r="C5" s="13">
         <v>-15.323700000000001</v>
       </c>
-      <c r="C5" s="13">
+      <c r="D5" s="13">
         <v>-12.789099999999999</v>
       </c>
-      <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="13">
+      <c r="C6" s="13">
         <v>-4.3</v>
       </c>
-      <c r="C6" s="13">
+      <c r="D6" s="13">
         <v>1.6</v>
       </c>
-      <c r="D6" s="13">
+      <c r="E6" s="13">
         <v>-11.5</v>
       </c>
-      <c r="E6" s="13">
+      <c r="F6" s="13">
         <v>-0.8</v>
       </c>
-      <c r="F6" s="13">
+      <c r="G6" s="13">
         <v>-2.5</v>
       </c>
-      <c r="G6" s="13">
+      <c r="H6" s="13">
         <v>-4.2</v>
       </c>
-      <c r="H6" s="13">
+      <c r="I6" s="13">
         <v>-0.5</v>
       </c>
-      <c r="I6" s="13">
+      <c r="J6" s="13">
         <v>-1.3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="13">
+      <c r="C7" s="13">
         <v>-3.5659999999999998</v>
       </c>
-      <c r="C7" s="13">
+      <c r="D7" s="13">
         <v>-0.5968</v>
       </c>
-      <c r="D7" s="13">
+      <c r="E7" s="13">
         <v>-10.3956</v>
       </c>
-      <c r="E7" s="13">
+      <c r="F7" s="13">
         <v>-2.4392</v>
       </c>
-      <c r="F7" s="13">
+      <c r="G7" s="13">
         <v>4.7607999999999997</v>
       </c>
-      <c r="G7" s="13">
+      <c r="H7" s="13">
         <v>-4.1600999999999999</v>
       </c>
-      <c r="H7" s="13">
+      <c r="I7" s="13">
         <v>-2.0428999999999999</v>
       </c>
-      <c r="I7" s="13">
+      <c r="J7" s="13">
         <v>-0.38080000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="13">
+      <c r="C8" s="13">
         <v>-4.9553000000000003</v>
       </c>
-      <c r="C8" s="14">
+      <c r="D8" s="14">
         <v>6.1597E+18</v>
       </c>
-      <c r="D8" s="13">
+      <c r="E8" s="13">
         <v>-13.9963</v>
       </c>
-      <c r="E8" s="14">
+      <c r="F8" s="14">
         <v>3.4736999999999997E+45</v>
       </c>
-      <c r="F8" s="13">
+      <c r="G8" s="13">
         <v>-2.9847000000000001</v>
       </c>
-      <c r="G8" s="13">
+      <c r="H8" s="13">
         <v>-4.5688000000000004</v>
       </c>
-      <c r="H8" s="13">
+      <c r="I8" s="13">
         <v>-1.6102000000000001</v>
       </c>
-      <c r="I8" s="14">
+      <c r="J8" s="14">
         <v>2.8743999999999999E+44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16">
+      <c r="C9" s="15"/>
+      <c r="D9" s="16">
         <v>4.7473000000000001</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16">
+      <c r="E9" s="15"/>
+      <c r="F9" s="16">
         <v>161.745</v>
       </c>
-      <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
-      <c r="I9" s="16">
+      <c r="I9" s="15"/>
+      <c r="J9" s="16">
         <v>177.05170000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="18">
+        <v>-2.4333999999999998</v>
+      </c>
+      <c r="D15" s="18">
+        <v>0.39710000000000001</v>
+      </c>
+      <c r="E15" s="18">
+        <v>-1.4021999999999999</v>
+      </c>
+      <c r="F15" s="18">
+        <v>0.90859999999999996</v>
+      </c>
+      <c r="G15" s="18">
+        <v>-0.23330000000000001</v>
+      </c>
+      <c r="H15" s="18">
+        <v>-0.3029</v>
+      </c>
+      <c r="I15" s="18">
+        <v>-0.14630000000000001</v>
+      </c>
+      <c r="J15" s="18">
+        <v>7.0800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="18">
+        <v>-4.5010000000000003</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-1.5115000000000001</v>
+      </c>
+      <c r="E16" s="18">
+        <v>-1.7454000000000001</v>
+      </c>
+      <c r="F16" s="18">
+        <v>-2.09</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0.94450000000000001</v>
+      </c>
+      <c r="H16" s="18">
+        <v>-0.66759999999999997</v>
+      </c>
+      <c r="I16" s="18">
+        <v>0.44950000000000001</v>
+      </c>
+      <c r="J16" s="18">
+        <v>-0.1013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="20">
+        <v>-1.9511000000000001</v>
+      </c>
+      <c r="D17" s="19">
+        <v>0.40229999999999999</v>
+      </c>
+      <c r="E17" s="18">
+        <v>-1.2970999999999999</v>
+      </c>
+      <c r="F17" s="18">
+        <v>0.60670000000000002</v>
+      </c>
+      <c r="G17" s="18">
+        <v>-0.27260000000000001</v>
+      </c>
+      <c r="H17" s="18">
+        <v>-0.33079999999999998</v>
+      </c>
+      <c r="I17" s="18">
+        <v>-0.15629999999999999</v>
+      </c>
+      <c r="J17" s="18">
+        <v>-9.2799999999999994E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="19">
+        <v>0.33189999999999997</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19">
+        <v>15.1043</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19">
+        <v>2.1004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="23">
+        <v>7470400000</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23">
+        <v>6.6192999999999997E+46</v>
+      </c>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23">
+        <v>5.4772000000000002E+45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19">
+        <v>0.29830000000000001</v>
+      </c>
+      <c r="E22" s="19">
+        <v>-1.2559</v>
+      </c>
+      <c r="F22" s="19">
+        <v>5.1799999999999999E-2</v>
+      </c>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19">
+        <v>-0.12920000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="19">
+        <v>0.47420000000000001</v>
+      </c>
+      <c r="E23" s="19">
+        <v>-1.3398000000000001</v>
+      </c>
+      <c r="F23" s="19">
+        <v>0.57679999999999998</v>
+      </c>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19">
+        <v>-0.11890000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="19">
+        <v>-2.0199999999999999E-2</v>
+      </c>
+      <c r="E26" s="19">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="F26" s="19">
+        <v>1.5696000000000001</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19">
+        <v>0.82250000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19">
+        <v>0.34549999999999997</v>
+      </c>
+      <c r="E27" s="19">
+        <v>-2.5206</v>
+      </c>
+      <c r="F27" s="19">
+        <v>212.93270000000001</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19">
+        <v>16.874300000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1 d time step advect
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14620" yWindow="460" windowWidth="16740" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="12060" yWindow="460" windowWidth="16740" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>Case</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>Old-13</t>
+  </si>
+  <si>
+    <t>New 200m transport /12,  vel/depth in flux calc, dt = 1 d, j = 2</t>
   </si>
 </sst>
 </file>
@@ -642,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,111 +1045,115 @@
         <v>-9.2799999999999994E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="4"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="21"/>
+      <c r="B18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="20">
+        <v>-0.31659999999999999</v>
+      </c>
+      <c r="D18" s="19">
+        <v>3.1899999999999998E-2</v>
+      </c>
       <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
+      <c r="F18" s="18">
+        <v>7.3300000000000004E-2</v>
+      </c>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-    </row>
-    <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="15">
-        <v>14</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="18">
-        <v>-3.5659999999999998</v>
-      </c>
-      <c r="D19" s="18">
-        <v>-0.5968</v>
-      </c>
-      <c r="E19" s="18">
-        <v>-10.3956</v>
-      </c>
-      <c r="F19" s="18">
-        <v>-2.4392</v>
-      </c>
-      <c r="G19" s="18">
-        <v>4.7607999999999997</v>
-      </c>
-      <c r="H19" s="18">
-        <v>-4.1600999999999999</v>
-      </c>
-      <c r="I19" s="18">
-        <v>-2.0428999999999999</v>
-      </c>
-      <c r="J19" s="18">
-        <v>-0.38080000000000003</v>
-      </c>
+      <c r="J18" s="18">
+        <v>-1.5900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
     </row>
     <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="18">
-        <v>-4.9553000000000003</v>
-      </c>
-      <c r="D20" s="9">
-        <v>6.1597E+18</v>
-      </c>
-      <c r="E20" s="8">
-        <v>-13.9963</v>
-      </c>
-      <c r="F20" s="9">
-        <v>3.4736999999999997E+45</v>
-      </c>
-      <c r="G20" s="8">
-        <v>-2.9847000000000001</v>
-      </c>
-      <c r="H20" s="10">
-        <v>-4.5688000000000004</v>
-      </c>
-      <c r="I20" s="8">
-        <v>-1.6102000000000001</v>
-      </c>
-      <c r="J20" s="9">
-        <v>2.8743999999999999E+44</v>
+        <v>-3.5659999999999998</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-0.5968</v>
+      </c>
+      <c r="E20" s="18">
+        <v>-10.3956</v>
+      </c>
+      <c r="F20" s="18">
+        <v>-2.4392</v>
+      </c>
+      <c r="G20" s="18">
+        <v>4.7607999999999997</v>
+      </c>
+      <c r="H20" s="18">
+        <v>-4.1600999999999999</v>
+      </c>
+      <c r="I20" s="18">
+        <v>-2.0428999999999999</v>
+      </c>
+      <c r="J20" s="18">
+        <v>-0.38080000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="19">
-        <v>-2.4392</v>
-      </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="C21" s="18">
+        <v>-4.9553000000000003</v>
+      </c>
+      <c r="D21" s="9">
+        <v>6.1597E+18</v>
+      </c>
+      <c r="E21" s="8">
+        <v>-13.9963</v>
+      </c>
+      <c r="F21" s="9">
+        <v>3.4736999999999997E+45</v>
+      </c>
+      <c r="G21" s="8">
+        <v>-2.9847000000000001</v>
+      </c>
+      <c r="H21" s="10">
+        <v>-4.5688000000000004</v>
+      </c>
+      <c r="I21" s="8">
+        <v>-1.6102000000000001</v>
+      </c>
+      <c r="J21" s="9">
+        <v>2.8743999999999999E+44</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="7">
-        <v>3.4736999999999997E+45</v>
+      <c r="F22" s="19">
+        <v>-2.4392</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -1155,116 +1162,116 @@
     </row>
     <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="15">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="7">
-        <v>2.6601999999999998E+37</v>
-      </c>
+      <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="7">
-        <v>3.1471000000000002E+46</v>
+        <v>3.4736999999999997E+45</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="7">
-        <v>1.5424999999999999E+42</v>
-      </c>
+      <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="15">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="6"/>
-      <c r="D24" s="19">
-        <v>4.7473000000000001</v>
-      </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19">
-        <v>161.745</v>
-      </c>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19">
-        <v>177.05170000000001</v>
+      <c r="D24" s="7">
+        <v>2.6601999999999998E+37</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7">
+        <v>3.1471000000000002E+46</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="7">
+        <v>1.5424999999999999E+42</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="15">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="19">
-        <v>0.33189999999999997</v>
+        <v>4.7473000000000001</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="19">
-        <v>15.1043</v>
+        <v>161.745</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
       <c r="I25" s="19"/>
       <c r="J25" s="19">
-        <v>2.1004</v>
+        <v>177.05170000000001</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="15">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="6"/>
-      <c r="D26" s="7">
-        <v>7470400000</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7">
-        <v>6.6192999999999997E+46</v>
-      </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="7">
-        <v>5.4772000000000002E+45</v>
+      <c r="D26" s="19">
+        <v>0.33189999999999997</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19">
+        <v>15.1043</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19">
+        <v>2.1004</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="7">
+        <v>7470400000</v>
+      </c>
       <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="F27" s="7">
+        <v>6.6192999999999997E+46</v>
+      </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="7">
-        <v>2.2199000000000001E+46</v>
+        <v>5.4772000000000002E+45</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="15">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -1273,183 +1280,201 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
-      <c r="J28" s="19">
+      <c r="J28" s="7">
+        <v>2.2199000000000001E+46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="15">
+        <v>23</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="19">
         <v>44.083599999999997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="21">
-        <v>25</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="19">
-        <v>-1.8743000000000001</v>
-      </c>
-      <c r="D29" s="19">
-        <v>0.29830000000000001</v>
-      </c>
-      <c r="E29" s="19">
-        <v>-1.2559</v>
-      </c>
-      <c r="F29" s="19">
-        <v>5.1799999999999999E-2</v>
-      </c>
-      <c r="G29" s="19">
-        <v>-0.23230000000000001</v>
-      </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19">
-        <v>-0.12920000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="21">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C30" s="19">
-        <v>-2.0024000000000002</v>
+        <v>-1.8743000000000001</v>
       </c>
       <c r="D30" s="19">
-        <v>0.47420000000000001</v>
+        <v>0.29830000000000001</v>
       </c>
       <c r="E30" s="19">
-        <v>-1.3398000000000001</v>
+        <v>-1.2559</v>
       </c>
       <c r="F30" s="19">
-        <v>0.57679999999999998</v>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="G30" s="19">
-        <v>-0.31090000000000001</v>
+        <v>-0.23230000000000001</v>
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19">
+        <v>-0.12920000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="21">
+        <v>26</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="19">
+        <v>-2.0024000000000002</v>
+      </c>
+      <c r="D31" s="19">
+        <v>0.47420000000000001</v>
+      </c>
+      <c r="E31" s="19">
+        <v>-1.3398000000000001</v>
+      </c>
+      <c r="F31" s="19">
+        <v>0.57679999999999998</v>
+      </c>
+      <c r="G31" s="19">
+        <v>-0.31090000000000001</v>
+      </c>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19">
         <v>-0.11890000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="21">
-        <v>27</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="19">
-        <v>-2.0199999999999999E-2</v>
-      </c>
-      <c r="E34" s="19">
-        <v>1.0800000000000001E-2</v>
-      </c>
-      <c r="F34" s="19">
-        <v>1.5696000000000001</v>
-      </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19">
-        <v>0.82250000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="21">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" s="19"/>
+        <v>53</v>
+      </c>
       <c r="D35" s="19">
-        <v>0.34549999999999997</v>
+        <v>-2.0199999999999999E-2</v>
       </c>
       <c r="E35" s="19">
-        <v>-2.5206</v>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="F35" s="19">
-        <v>212.93270000000001</v>
+        <v>1.5696000000000001</v>
       </c>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19">
+        <v>0.82250000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="21">
+        <v>28</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19">
+        <v>0.34549999999999997</v>
+      </c>
+      <c r="E36" s="19">
+        <v>-2.5206</v>
+      </c>
+      <c r="F36" s="19">
+        <v>212.93270000000001</v>
+      </c>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19">
         <v>16.874300000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="3" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B46" s="3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="1">
-        <v>5.7000000000000005E+95</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C47" s="1">
-        <v>1.2E+106</v>
+        <v>5.7000000000000005E+95</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C48" s="1">
-        <v>4.4000000000000004E+93</v>
+        <v>1.2E+106</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C49" s="1">
-        <v>2700000000</v>
+        <v>4.4000000000000004E+93</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C50" s="1">
-        <v>91000000</v>
+        <v>2700000000</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C51" s="1">
-        <v>2500</v>
+        <v>91000000</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B53" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C53" s="1">
         <v>9.5999999999999996E+83</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D53" s="1">
         <v>1.2999999999999999E+24</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E53" s="1">
         <v>4.6000000000000003E+93</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F53" s="1">
         <v>7.4999999999999994E+29</v>
       </c>
-      <c r="G52" s="1">
+      <c r="G53" s="1">
         <v>37.9</v>
       </c>
     </row>

</xml_diff>